<commit_message>
Filled out the time table
</commit_message>
<xml_diff>
--- a/Documents/Table.xlsx
+++ b/Documents/Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mega_chungus_linux\Code\Operating Systems\CSCI-474-Project1\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\medium_chungus_linux\Coding\Operating Systems Code\CSCI-474-Project1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856E7C76-C0E4-4EA8-9A77-C555EE38E371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F978A91-C460-4C4C-B6F6-C5E457F8533B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{13FD98BF-07EE-4C27-ADAF-EF0E8AD80A94}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{13FD98BF-07EE-4C27-ADAF-EF0E8AD80A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>File 1</t>
   </si>
@@ -65,9 +65,6 @@
     <t>4 Processes</t>
   </si>
   <si>
-    <t>Time taken (sec)</t>
-  </si>
-  <si>
     <t>File name</t>
   </si>
   <si>
@@ -78,6 +75,21 @@
   </si>
   <si>
     <t>100,000 lines</t>
+  </si>
+  <si>
+    <t>Time taken (ms)</t>
+  </si>
+  <si>
+    <t>Test 4</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t>File 2</t>
+  </si>
+  <si>
+    <t>File 3</t>
   </si>
 </sst>
 </file>
@@ -508,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974E4C39-6E02-4057-A847-8F6AE1FBA4B8}">
-  <dimension ref="B2:G12"/>
+  <dimension ref="B2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,17 +532,19 @@
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -545,141 +559,255 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="e">
-        <f>AVERAGE(D4:F4)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I4" s="1">
+        <f>AVERAGE(D4:H4)</f>
+        <v>0.78239999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="e">
-        <f t="shared" ref="G5:G6" si="0">AVERAGE(D5:F5)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.874</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.876</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" ref="I5:I12" si="0">AVERAGE(D5:H5)</f>
+        <v>0.89300000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="e">
+      <c r="D6" s="1">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.129</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.1759999999999999</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>1.0946</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="e">
-        <f>AVERAGE(D7:F7)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>3.3969999999999998</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.3940000000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3.3460000000000001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3.3570000000000002</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3868</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="e">
-        <f t="shared" ref="G8:G9" si="1">AVERAGE(D8:F8)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.2149999999999999</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.0609999999999999</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2.137</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1616</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.63</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.7150000000000001</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1.6779999999999999</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.625</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6846000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="e">
-        <f>AVERAGE(D10:F10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4.7160000000000002</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4.92</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4.8929999999999998</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4.8449999999999998</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8628</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="e">
-        <f t="shared" ref="G11:G12" si="2">AVERAGE(D11:F11)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>2.6230000000000002</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.61</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.5979999999999999</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.5670000000000002</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5815999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D12" s="1">
+        <v>1.502</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.5129999999999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1.448</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.4019999999999999</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.476</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>